<commit_message>
Remove warnings import from numpy
</commit_message>
<xml_diff>
--- a/dev/Input data_tw.xlsx
+++ b/dev/Input data_tw.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="10811"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="10112"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/romain/Github/carculator_two_wheeler/dev/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1946D27A-E08E-EA47-9525-705A33EE5F8F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0233662E-37E7-0D47-9555-3EE641D6A6BD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="760" windowWidth="22040" windowHeight="22720" tabRatio="518" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="5260" yWindow="660" windowWidth="22040" windowHeight="22720" tabRatio="518" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Vehicle parameters" sheetId="22" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1798" uniqueCount="222">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1822" uniqueCount="225">
   <si>
     <t>power to mass ratio</t>
   </si>
@@ -703,6 +703,15 @@
   </si>
   <si>
     <t>battery cycle life, NMC-955</t>
+  </si>
+  <si>
+    <t>battery cycle life, Li-O2</t>
+  </si>
+  <si>
+    <t>battery cycle life, Li-S</t>
+  </si>
+  <si>
+    <t>battery cycle life, SiB</t>
   </si>
 </sst>
 </file>
@@ -1177,13 +1186,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:AT200"/>
+  <dimension ref="A1:AT203"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
       <pane xSplit="10" ySplit="2" topLeftCell="Y164" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="F1" sqref="F1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="D209" sqref="D209"/>
+      <selection pane="bottomRight" activeCell="G167" sqref="G167"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.33203125" defaultRowHeight="14" x14ac:dyDescent="0.2"/>
@@ -19439,6 +19448,264 @@
         <v>5000</v>
       </c>
     </row>
+    <row r="201" spans="1:28" x14ac:dyDescent="0.2">
+      <c r="A201" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="B201" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="C201" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="D201" s="3" t="s">
+        <v>222</v>
+      </c>
+      <c r="E201" s="3" t="s">
+        <v>36</v>
+      </c>
+      <c r="F201" s="3" t="s">
+        <v>31</v>
+      </c>
+      <c r="G201" s="3"/>
+      <c r="H201" s="3"/>
+      <c r="I201" s="3" t="s">
+        <v>54</v>
+      </c>
+      <c r="J201" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="K201" s="5">
+        <v>1300</v>
+      </c>
+      <c r="L201" s="5">
+        <v>1000</v>
+      </c>
+      <c r="M201" s="5">
+        <v>1500</v>
+      </c>
+      <c r="N201" s="5">
+        <v>1300</v>
+      </c>
+      <c r="O201" s="5">
+        <v>1000</v>
+      </c>
+      <c r="P201" s="5">
+        <v>1500</v>
+      </c>
+      <c r="Q201" s="5">
+        <v>1300</v>
+      </c>
+      <c r="R201" s="5">
+        <v>1000</v>
+      </c>
+      <c r="S201" s="5">
+        <v>1500</v>
+      </c>
+      <c r="T201" s="5">
+        <v>1300</v>
+      </c>
+      <c r="U201" s="5">
+        <v>1000</v>
+      </c>
+      <c r="V201" s="5">
+        <v>1500</v>
+      </c>
+      <c r="W201" s="5">
+        <v>1300</v>
+      </c>
+      <c r="X201" s="5">
+        <v>1000</v>
+      </c>
+      <c r="Y201" s="5">
+        <v>1500</v>
+      </c>
+      <c r="Z201" s="5">
+        <v>1300</v>
+      </c>
+      <c r="AA201" s="5">
+        <v>1000</v>
+      </c>
+      <c r="AB201" s="5">
+        <v>1500</v>
+      </c>
+    </row>
+    <row r="202" spans="1:28" x14ac:dyDescent="0.2">
+      <c r="A202" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="B202" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="C202" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="D202" s="3" t="s">
+        <v>223</v>
+      </c>
+      <c r="E202" s="3" t="s">
+        <v>36</v>
+      </c>
+      <c r="F202" s="3" t="s">
+        <v>31</v>
+      </c>
+      <c r="G202" s="3"/>
+      <c r="H202" s="3"/>
+      <c r="I202" s="3" t="s">
+        <v>54</v>
+      </c>
+      <c r="J202" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="K202" s="5">
+        <f>AVERAGE(L202,M202)</f>
+        <v>1150</v>
+      </c>
+      <c r="L202" s="5">
+        <v>800</v>
+      </c>
+      <c r="M202" s="5">
+        <v>1500</v>
+      </c>
+      <c r="N202" s="5">
+        <f>AVERAGE(O202,P202)</f>
+        <v>1150</v>
+      </c>
+      <c r="O202" s="5">
+        <v>800</v>
+      </c>
+      <c r="P202" s="5">
+        <v>1500</v>
+      </c>
+      <c r="Q202" s="5">
+        <f>AVERAGE(R202,S202)</f>
+        <v>1150</v>
+      </c>
+      <c r="R202" s="5">
+        <v>800</v>
+      </c>
+      <c r="S202" s="5">
+        <v>1500</v>
+      </c>
+      <c r="T202" s="5">
+        <f>AVERAGE(U202,V202)</f>
+        <v>1150</v>
+      </c>
+      <c r="U202" s="5">
+        <v>800</v>
+      </c>
+      <c r="V202" s="5">
+        <v>1500</v>
+      </c>
+      <c r="W202" s="5">
+        <f>AVERAGE(X202,Y202)</f>
+        <v>1150</v>
+      </c>
+      <c r="X202" s="5">
+        <v>800</v>
+      </c>
+      <c r="Y202" s="5">
+        <v>1500</v>
+      </c>
+      <c r="Z202" s="5">
+        <f>AVERAGE(AA202,AB202)</f>
+        <v>1150</v>
+      </c>
+      <c r="AA202" s="5">
+        <v>800</v>
+      </c>
+      <c r="AB202" s="5">
+        <v>1500</v>
+      </c>
+    </row>
+    <row r="203" spans="1:28" x14ac:dyDescent="0.2">
+      <c r="A203" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="B203" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="C203" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="D203" s="3" t="s">
+        <v>224</v>
+      </c>
+      <c r="E203" s="3" t="s">
+        <v>36</v>
+      </c>
+      <c r="F203" s="3" t="s">
+        <v>31</v>
+      </c>
+      <c r="G203" s="3"/>
+      <c r="H203" s="3"/>
+      <c r="I203" s="3" t="s">
+        <v>54</v>
+      </c>
+      <c r="J203" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="K203" s="5">
+        <f>AVERAGE(L203,M203)</f>
+        <v>3250</v>
+      </c>
+      <c r="L203" s="5">
+        <v>2500</v>
+      </c>
+      <c r="M203" s="5">
+        <v>4000</v>
+      </c>
+      <c r="N203" s="5">
+        <f>AVERAGE(O203,P203)</f>
+        <v>3250</v>
+      </c>
+      <c r="O203" s="5">
+        <v>2500</v>
+      </c>
+      <c r="P203" s="5">
+        <v>4000</v>
+      </c>
+      <c r="Q203" s="5">
+        <f>AVERAGE(R203,S203)</f>
+        <v>3250</v>
+      </c>
+      <c r="R203" s="5">
+        <v>2500</v>
+      </c>
+      <c r="S203" s="5">
+        <v>4000</v>
+      </c>
+      <c r="T203" s="5">
+        <f>AVERAGE(U203,V203)</f>
+        <v>3250</v>
+      </c>
+      <c r="U203" s="5">
+        <v>2500</v>
+      </c>
+      <c r="V203" s="5">
+        <v>4000</v>
+      </c>
+      <c r="W203" s="5">
+        <f>AVERAGE(X203,Y203)</f>
+        <v>3250</v>
+      </c>
+      <c r="X203" s="5">
+        <v>2500</v>
+      </c>
+      <c r="Y203" s="5">
+        <v>4000</v>
+      </c>
+      <c r="Z203" s="5">
+        <f>AVERAGE(AA203,AB203)</f>
+        <v>3250</v>
+      </c>
+      <c r="AA203" s="5">
+        <v>2500</v>
+      </c>
+      <c r="AB203" s="5">
+        <v>4000</v>
+      </c>
+    </row>
   </sheetData>
   <autoFilter ref="A2:AB192" xr:uid="{00000000-0009-0000-0000-000000000000}"/>
   <phoneticPr fontId="9" type="noConversion"/>

</xml_diff>